<commit_message>
Counts of Acts enforced by the regs in scope
</commit_message>
<xml_diff>
--- a/Regs_Acts_Counts_v1.xlsx
+++ b/Regs_Acts_Counts_v1.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A.R.Wong\Desktop\GitHub\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{705E8FC7-3370-49EC-9987-A9F38D11759E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1111,8 +1117,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1175,6 +1181,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1221,7 +1235,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1253,9 +1267,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1287,6 +1319,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1462,19 +1512,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B364"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1482,7 +1534,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1490,7 +1542,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1498,7 +1550,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1506,7 +1558,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1514,7 +1566,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1522,7 +1574,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1530,7 +1582,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1538,7 +1590,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1546,7 +1598,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1554,7 +1606,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1562,7 +1614,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1570,7 +1622,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1578,7 +1630,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1586,7 +1638,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1594,7 +1646,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1602,7 +1654,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1610,7 +1662,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1618,7 +1670,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1626,7 +1678,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1634,7 +1686,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1642,7 +1694,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1650,7 +1702,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1658,7 +1710,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1666,7 +1718,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1674,7 +1726,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1682,7 +1734,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -1690,7 +1742,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1698,7 +1750,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -1706,7 +1758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -1714,7 +1766,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -1722,7 +1774,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -1730,7 +1782,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -1738,7 +1790,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -1746,7 +1798,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -1754,7 +1806,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -1762,7 +1814,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -1770,7 +1822,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -1778,7 +1830,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -1786,7 +1838,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -1794,7 +1846,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -1802,7 +1854,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -1810,7 +1862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
@@ -1818,7 +1870,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
@@ -1826,7 +1878,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
@@ -1834,7 +1886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
@@ -1842,7 +1894,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
@@ -1850,7 +1902,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
@@ -1858,7 +1910,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
@@ -1866,7 +1918,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
@@ -1874,7 +1926,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
@@ -1882,7 +1934,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
@@ -1890,7 +1942,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
@@ -1898,7 +1950,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
@@ -1906,7 +1958,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
@@ -1914,7 +1966,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
@@ -1922,7 +1974,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
@@ -1930,7 +1982,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
@@ -1938,7 +1990,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
@@ -1946,7 +1998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
@@ -1954,7 +2006,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
@@ -1962,7 +2014,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
@@ -1970,7 +2022,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
@@ -1978,7 +2030,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
@@ -1986,7 +2038,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
@@ -1994,7 +2046,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
@@ -2002,7 +2054,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
@@ -2010,7 +2062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
@@ -2018,7 +2070,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
@@ -2026,7 +2078,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
@@ -2034,7 +2086,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
@@ -2042,7 +2094,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
@@ -2050,7 +2102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>73</v>
       </c>
@@ -2058,7 +2110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
@@ -2066,7 +2118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>75</v>
       </c>
@@ -2074,7 +2126,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
@@ -2082,7 +2134,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>77</v>
       </c>
@@ -2090,7 +2142,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>78</v>
       </c>
@@ -2098,7 +2150,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>79</v>
       </c>
@@ -2106,7 +2158,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>80</v>
       </c>
@@ -2114,7 +2166,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>81</v>
       </c>
@@ -2122,7 +2174,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>82</v>
       </c>
@@ -2130,7 +2182,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>83</v>
       </c>
@@ -2138,7 +2190,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>84</v>
       </c>
@@ -2146,7 +2198,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>85</v>
       </c>
@@ -2154,7 +2206,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>86</v>
       </c>
@@ -2162,7 +2214,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>87</v>
       </c>
@@ -2170,7 +2222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>88</v>
       </c>
@@ -2178,7 +2230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>89</v>
       </c>
@@ -2186,7 +2238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>90</v>
       </c>
@@ -2194,7 +2246,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>91</v>
       </c>
@@ -2202,7 +2254,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
@@ -2210,7 +2262,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>93</v>
       </c>
@@ -2218,7 +2270,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>94</v>
       </c>
@@ -2226,7 +2278,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>95</v>
       </c>
@@ -2234,7 +2286,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>96</v>
       </c>
@@ -2242,7 +2294,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>97</v>
       </c>
@@ -2250,7 +2302,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>98</v>
       </c>
@@ -2258,7 +2310,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>99</v>
       </c>
@@ -2266,7 +2318,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>100</v>
       </c>
@@ -2274,7 +2326,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>101</v>
       </c>
@@ -2282,7 +2334,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>102</v>
       </c>
@@ -2290,7 +2342,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>103</v>
       </c>
@@ -2298,7 +2350,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>104</v>
       </c>
@@ -2306,7 +2358,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>105</v>
       </c>
@@ -2314,7 +2366,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>106</v>
       </c>
@@ -2322,7 +2374,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>107</v>
       </c>
@@ -2330,7 +2382,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>108</v>
       </c>
@@ -2338,7 +2390,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>109</v>
       </c>
@@ -2346,7 +2398,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>110</v>
       </c>
@@ -2354,7 +2406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>111</v>
       </c>
@@ -2362,7 +2414,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>112</v>
       </c>
@@ -2370,7 +2422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>113</v>
       </c>
@@ -2378,7 +2430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>114</v>
       </c>
@@ -2386,7 +2438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>115</v>
       </c>
@@ -2394,7 +2446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>116</v>
       </c>
@@ -2402,7 +2454,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>117</v>
       </c>
@@ -2410,7 +2462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>118</v>
       </c>
@@ -2418,7 +2470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>119</v>
       </c>
@@ -2426,7 +2478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>120</v>
       </c>
@@ -2434,7 +2486,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>121</v>
       </c>
@@ -2442,7 +2494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>122</v>
       </c>
@@ -2450,7 +2502,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>123</v>
       </c>
@@ -2458,7 +2510,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>124</v>
       </c>
@@ -2466,7 +2518,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>125</v>
       </c>
@@ -2474,7 +2526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>126</v>
       </c>
@@ -2482,7 +2534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>127</v>
       </c>
@@ -2490,7 +2542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>128</v>
       </c>
@@ -2498,7 +2550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>129</v>
       </c>
@@ -2506,7 +2558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>130</v>
       </c>
@@ -2514,7 +2566,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>131</v>
       </c>
@@ -2522,7 +2574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>132</v>
       </c>
@@ -2530,7 +2582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>133</v>
       </c>
@@ -2538,7 +2590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>134</v>
       </c>
@@ -2546,7 +2598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>135</v>
       </c>
@@ -2554,7 +2606,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>136</v>
       </c>
@@ -2562,7 +2614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>137</v>
       </c>
@@ -2570,7 +2622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>138</v>
       </c>
@@ -2578,7 +2630,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>139</v>
       </c>
@@ -2586,7 +2638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>140</v>
       </c>
@@ -2594,7 +2646,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>141</v>
       </c>
@@ -2602,7 +2654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>142</v>
       </c>
@@ -2610,7 +2662,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>143</v>
       </c>
@@ -2618,7 +2670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>144</v>
       </c>
@@ -2626,7 +2678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>145</v>
       </c>
@@ -2634,7 +2686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>146</v>
       </c>
@@ -2642,7 +2694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>147</v>
       </c>
@@ -2650,7 +2702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>148</v>
       </c>
@@ -2658,7 +2710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>149</v>
       </c>
@@ -2666,7 +2718,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>150</v>
       </c>
@@ -2674,7 +2726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>151</v>
       </c>
@@ -2682,7 +2734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>152</v>
       </c>
@@ -2690,7 +2742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>153</v>
       </c>
@@ -2698,7 +2750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>154</v>
       </c>
@@ -2706,7 +2758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>155</v>
       </c>
@@ -2714,7 +2766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>156</v>
       </c>
@@ -2722,7 +2774,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>157</v>
       </c>
@@ -2730,7 +2782,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>158</v>
       </c>
@@ -2738,7 +2790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>159</v>
       </c>
@@ -2746,7 +2798,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>160</v>
       </c>
@@ -2754,7 +2806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>161</v>
       </c>
@@ -2762,7 +2814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>162</v>
       </c>
@@ -2770,7 +2822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>163</v>
       </c>
@@ -2778,7 +2830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>164</v>
       </c>
@@ -2786,7 +2838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>165</v>
       </c>
@@ -2794,7 +2846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>166</v>
       </c>
@@ -2802,7 +2854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>167</v>
       </c>
@@ -2810,7 +2862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>168</v>
       </c>
@@ -2818,7 +2870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>169</v>
       </c>
@@ -2826,7 +2878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>170</v>
       </c>
@@ -2834,7 +2886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>171</v>
       </c>
@@ -2842,7 +2894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>172</v>
       </c>
@@ -2850,7 +2902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>173</v>
       </c>
@@ -2858,7 +2910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>174</v>
       </c>
@@ -2866,7 +2918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>175</v>
       </c>
@@ -2874,7 +2926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>176</v>
       </c>
@@ -2882,7 +2934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>177</v>
       </c>
@@ -2890,7 +2942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>178</v>
       </c>
@@ -2898,7 +2950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>179</v>
       </c>
@@ -2906,7 +2958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>180</v>
       </c>
@@ -2914,7 +2966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>181</v>
       </c>
@@ -2922,7 +2974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>182</v>
       </c>
@@ -2930,7 +2982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>183</v>
       </c>
@@ -2938,7 +2990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>184</v>
       </c>
@@ -2946,7 +2998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>185</v>
       </c>
@@ -2954,7 +3006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>186</v>
       </c>
@@ -2962,7 +3014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>187</v>
       </c>
@@ -2970,7 +3022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>188</v>
       </c>
@@ -2978,7 +3030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>189</v>
       </c>
@@ -2986,7 +3038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>190</v>
       </c>
@@ -2994,7 +3046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>191</v>
       </c>
@@ -3002,7 +3054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>192</v>
       </c>
@@ -3010,7 +3062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>193</v>
       </c>
@@ -3018,7 +3070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>194</v>
       </c>
@@ -3026,7 +3078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>195</v>
       </c>
@@ -3034,7 +3086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>196</v>
       </c>
@@ -3042,7 +3094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:2">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>197</v>
       </c>
@@ -3050,7 +3102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>198</v>
       </c>
@@ -3058,7 +3110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>199</v>
       </c>
@@ -3066,7 +3118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>200</v>
       </c>
@@ -3074,7 +3126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>201</v>
       </c>
@@ -3082,7 +3134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>202</v>
       </c>
@@ -3090,7 +3142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>203</v>
       </c>
@@ -3098,7 +3150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>204</v>
       </c>
@@ -3106,7 +3158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>205</v>
       </c>
@@ -3114,7 +3166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>206</v>
       </c>
@@ -3122,7 +3174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>207</v>
       </c>
@@ -3130,7 +3182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:2">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>208</v>
       </c>
@@ -3138,7 +3190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>209</v>
       </c>
@@ -3146,7 +3198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:2">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>210</v>
       </c>
@@ -3154,7 +3206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>211</v>
       </c>
@@ -3162,7 +3214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:2">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>212</v>
       </c>
@@ -3170,7 +3222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:2">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>213</v>
       </c>
@@ -3178,7 +3230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:2">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>214</v>
       </c>
@@ -3186,7 +3238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:2">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>215</v>
       </c>
@@ -3194,7 +3246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:2">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>216</v>
       </c>
@@ -3202,7 +3254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:2">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>217</v>
       </c>
@@ -3210,7 +3262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:2">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>218</v>
       </c>
@@ -3218,7 +3270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:2">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>219</v>
       </c>
@@ -3226,7 +3278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:2">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>220</v>
       </c>
@@ -3234,7 +3286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:2">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>221</v>
       </c>
@@ -3242,7 +3294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:2">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>222</v>
       </c>
@@ -3250,7 +3302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:2">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>223</v>
       </c>
@@ -3258,7 +3310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:2">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>224</v>
       </c>
@@ -3266,7 +3318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:2">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>225</v>
       </c>
@@ -3274,7 +3326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:2">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>226</v>
       </c>
@@ -3282,7 +3334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:2">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>227</v>
       </c>
@@ -3290,7 +3342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:2">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>228</v>
       </c>
@@ -3298,7 +3350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:2">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>229</v>
       </c>
@@ -3306,7 +3358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:2">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>230</v>
       </c>
@@ -3314,7 +3366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:2">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>231</v>
       </c>
@@ -3322,7 +3374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:2">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>232</v>
       </c>
@@ -3330,7 +3382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:2">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>233</v>
       </c>
@@ -3338,7 +3390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:2">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>234</v>
       </c>
@@ -3346,7 +3398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:2">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>235</v>
       </c>
@@ -3354,7 +3406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:2">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>236</v>
       </c>
@@ -3362,7 +3414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:2">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>237</v>
       </c>
@@ -3370,7 +3422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:2">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>238</v>
       </c>
@@ -3378,7 +3430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:2">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>239</v>
       </c>
@@ -3386,7 +3438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:2">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>240</v>
       </c>
@@ -3394,7 +3446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:2">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>241</v>
       </c>
@@ -3402,7 +3454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:2">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>242</v>
       </c>
@@ -3410,7 +3462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:2">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>243</v>
       </c>
@@ -3418,7 +3470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:2">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>244</v>
       </c>
@@ -3426,7 +3478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:2">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>245</v>
       </c>
@@ -3434,7 +3486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:2">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>246</v>
       </c>
@@ -3442,7 +3494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:2">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>247</v>
       </c>
@@ -3450,7 +3502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:2">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>248</v>
       </c>
@@ -3458,7 +3510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:2">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>249</v>
       </c>
@@ -3466,7 +3518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:2">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>250</v>
       </c>
@@ -3474,7 +3526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:2">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>251</v>
       </c>
@@ -3482,7 +3534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:2">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>252</v>
       </c>
@@ -3490,7 +3542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:2">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>253</v>
       </c>
@@ -3498,7 +3550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:2">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>254</v>
       </c>
@@ -3506,7 +3558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:2">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>255</v>
       </c>
@@ -3514,7 +3566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:2">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>256</v>
       </c>
@@ -3522,7 +3574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:2">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>257</v>
       </c>
@@ -3530,7 +3582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:2">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>258</v>
       </c>
@@ -3538,7 +3590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:2">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>259</v>
       </c>
@@ -3546,7 +3598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:2">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>260</v>
       </c>
@@ -3554,7 +3606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:2">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>261</v>
       </c>
@@ -3562,7 +3614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:2">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>262</v>
       </c>
@@ -3570,7 +3622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:2">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>263</v>
       </c>
@@ -3578,7 +3630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:2">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>264</v>
       </c>
@@ -3586,7 +3638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:2">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>265</v>
       </c>
@@ -3594,7 +3646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:2">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>266</v>
       </c>
@@ -3602,7 +3654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:2">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>267</v>
       </c>
@@ -3610,7 +3662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:2">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>268</v>
       </c>
@@ -3618,7 +3670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:2">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>269</v>
       </c>
@@ -3626,7 +3678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:2">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>270</v>
       </c>
@@ -3634,7 +3686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:2">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>271</v>
       </c>
@@ -3642,7 +3694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:2">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>272</v>
       </c>
@@ -3650,7 +3702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:2">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>273</v>
       </c>
@@ -3658,7 +3710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:2">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>274</v>
       </c>
@@ -3666,7 +3718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:2">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>275</v>
       </c>
@@ -3674,7 +3726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:2">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>276</v>
       </c>
@@ -3682,7 +3734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:2">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>277</v>
       </c>
@@ -3690,7 +3742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:2">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>278</v>
       </c>
@@ -3698,7 +3750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:2">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>279</v>
       </c>
@@ -3706,7 +3758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:2">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>280</v>
       </c>
@@ -3714,7 +3766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:2">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>281</v>
       </c>
@@ -3722,7 +3774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:2">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>282</v>
       </c>
@@ -3730,7 +3782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:2">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>283</v>
       </c>
@@ -3738,7 +3790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:2">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>284</v>
       </c>
@@ -3746,7 +3798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:2">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>285</v>
       </c>
@@ -3754,7 +3806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:2">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>286</v>
       </c>
@@ -3762,7 +3814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:2">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>287</v>
       </c>
@@ -3770,7 +3822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:2">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>288</v>
       </c>
@@ -3778,7 +3830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:2">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>289</v>
       </c>
@@ -3786,7 +3838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:2">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>290</v>
       </c>
@@ -3794,7 +3846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:2">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>291</v>
       </c>
@@ -3802,7 +3854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:2">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>292</v>
       </c>
@@ -3810,7 +3862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:2">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>293</v>
       </c>
@@ -3818,7 +3870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:2">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>294</v>
       </c>
@@ -3826,7 +3878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:2">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>295</v>
       </c>
@@ -3834,7 +3886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:2">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>296</v>
       </c>
@@ -3842,7 +3894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:2">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>297</v>
       </c>
@@ -3850,7 +3902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:2">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>298</v>
       </c>
@@ -3858,7 +3910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:2">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>299</v>
       </c>
@@ -3866,7 +3918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:2">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>300</v>
       </c>
@@ -3874,7 +3926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:2">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>301</v>
       </c>
@@ -3882,7 +3934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:2">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>302</v>
       </c>
@@ -3890,7 +3942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:2">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>303</v>
       </c>
@@ -3898,7 +3950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:2">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
         <v>304</v>
       </c>
@@ -3906,7 +3958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:2">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>305</v>
       </c>
@@ -3914,7 +3966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:2">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
         <v>306</v>
       </c>
@@ -3922,7 +3974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:2">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>307</v>
       </c>
@@ -3930,7 +3982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:2">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
         <v>308</v>
       </c>
@@ -3938,7 +3990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:2">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
         <v>309</v>
       </c>
@@ -3946,7 +3998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:2">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
         <v>310</v>
       </c>
@@ -3954,7 +4006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:2">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
         <v>311</v>
       </c>
@@ -3962,7 +4014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:2">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
         <v>312</v>
       </c>
@@ -3970,7 +4022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:2">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
         <v>313</v>
       </c>
@@ -3978,7 +4030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:2">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
         <v>314</v>
       </c>
@@ -3986,7 +4038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:2">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
         <v>315</v>
       </c>
@@ -3994,7 +4046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:2">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
         <v>316</v>
       </c>
@@ -4002,7 +4054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:2">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
         <v>317</v>
       </c>
@@ -4010,7 +4062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:2">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
         <v>318</v>
       </c>
@@ -4018,7 +4070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:2">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
         <v>319</v>
       </c>
@@ -4026,7 +4078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:2">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
         <v>320</v>
       </c>
@@ -4034,7 +4086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:2">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
         <v>321</v>
       </c>
@@ -4042,7 +4094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:2">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
         <v>322</v>
       </c>
@@ -4050,7 +4102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:2">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>323</v>
       </c>
@@ -4058,7 +4110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:2">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
         <v>324</v>
       </c>
@@ -4066,7 +4118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:2">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
         <v>325</v>
       </c>
@@ -4074,7 +4126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:2">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
         <v>326</v>
       </c>
@@ -4082,7 +4134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:2">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
         <v>327</v>
       </c>
@@ -4090,7 +4142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:2">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
         <v>328</v>
       </c>
@@ -4098,7 +4150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:2">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
         <v>329</v>
       </c>
@@ -4106,7 +4158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:2">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
         <v>330</v>
       </c>
@@ -4114,7 +4166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:2">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
         <v>331</v>
       </c>
@@ -4122,7 +4174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:2">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
         <v>332</v>
       </c>
@@ -4130,7 +4182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:2">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
         <v>333</v>
       </c>
@@ -4138,7 +4190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:2">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
         <v>334</v>
       </c>
@@ -4146,7 +4198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:2">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
         <v>335</v>
       </c>
@@ -4154,7 +4206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:2">
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
         <v>336</v>
       </c>
@@ -4162,7 +4214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:2">
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
         <v>337</v>
       </c>
@@ -4170,7 +4222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:2">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
         <v>338</v>
       </c>
@@ -4178,7 +4230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:2">
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
         <v>339</v>
       </c>
@@ -4186,7 +4238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" spans="1:2">
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
         <v>340</v>
       </c>
@@ -4194,7 +4246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:2">
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
         <v>341</v>
       </c>
@@ -4202,7 +4254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:2">
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
         <v>342</v>
       </c>
@@ -4210,7 +4262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:2">
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
         <v>343</v>
       </c>
@@ -4218,7 +4270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:2">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
         <v>344</v>
       </c>
@@ -4226,7 +4278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:2">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
         <v>345</v>
       </c>
@@ -4234,7 +4286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:2">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
         <v>346</v>
       </c>
@@ -4242,7 +4294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" spans="1:2">
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>347</v>
       </c>
@@ -4250,7 +4302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:2">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
         <v>348</v>
       </c>
@@ -4258,7 +4310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="1:2">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
         <v>349</v>
       </c>
@@ -4266,7 +4318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" spans="1:2">
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
         <v>350</v>
       </c>
@@ -4274,7 +4326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:2">
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
         <v>351</v>
       </c>
@@ -4282,7 +4334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:2">
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
         <v>352</v>
       </c>
@@ -4290,7 +4342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="354" spans="1:2">
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
         <v>353</v>
       </c>
@@ -4298,7 +4350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" spans="1:2">
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
         <v>354</v>
       </c>
@@ -4306,7 +4358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:2">
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
         <v>355</v>
       </c>
@@ -4314,7 +4366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:2">
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
         <v>356</v>
       </c>
@@ -4322,7 +4374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:2">
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
         <v>357</v>
       </c>
@@ -4330,7 +4382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="1:2">
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
         <v>358</v>
       </c>
@@ -4338,7 +4390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:2">
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
         <v>359</v>
       </c>
@@ -4346,7 +4398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" spans="1:2">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
         <v>360</v>
       </c>
@@ -4354,7 +4406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" spans="1:2">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
         <v>361</v>
       </c>
@@ -4362,7 +4414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="363" spans="1:2">
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
         <v>362</v>
       </c>
@@ -4370,7 +4422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" spans="1:2">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
         <v>363</v>
       </c>
@@ -4380,5 +4432,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>